<commit_message>
Updated category IDs in import.sql
</commit_message>
<xml_diff>
--- a/mock_data/20_radku_testovacich_transakci.xlsx
+++ b/mock_data/20_radku_testovacich_transakci.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\moria\mock_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5364EAB-7C1A-446E-B307-B83EEF933153}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58E9F43-2DAE-42C9-A9E3-55BF312B405F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="554" xr2:uid="{AC6126E9-B026-468E-A5ED-F833BADB1704}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="554" xr2:uid="{AC6126E9-B026-468E-A5ED-F833BADB1704}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -327,9 +327,6 @@
     <t>Regiojet CZ</t>
   </si>
   <si>
-    <t>I'm Lovin' It</t>
-  </si>
-  <si>
     <t>Muj landlord</t>
   </si>
   <si>
@@ -346,6 +343,9 @@
   </si>
   <si>
     <t>PAYMENT_HOME</t>
+  </si>
+  <si>
+    <t>Im Lovin It</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -411,9 +411,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -766,39 +768,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43CA8FA-B653-44BA-B2F7-6BE6088458A7}">
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="11" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="8" max="11" width="15.109375" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" customWidth="1"/>
-    <col min="15" max="15" width="22.5703125" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" customWidth="1"/>
+    <col min="14" max="14" width="16.6640625" customWidth="1"/>
+    <col min="15" max="15" width="22.5546875" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" customWidth="1"/>
-    <col min="18" max="18" width="18.85546875" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" customWidth="1"/>
-    <col min="20" max="20" width="24.42578125" customWidth="1"/>
-    <col min="21" max="21" width="22.140625" customWidth="1"/>
-    <col min="22" max="22" width="24.42578125" customWidth="1"/>
-    <col min="23" max="23" width="20.5703125" customWidth="1"/>
-    <col min="24" max="24" width="23.5703125" customWidth="1"/>
-    <col min="25" max="25" width="10.85546875" customWidth="1"/>
-    <col min="26" max="26" width="9.85546875" customWidth="1"/>
-    <col min="27" max="28" width="19.42578125" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" customWidth="1"/>
+    <col min="18" max="18" width="18.88671875" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" customWidth="1"/>
+    <col min="20" max="20" width="24.44140625" customWidth="1"/>
+    <col min="21" max="21" width="22.109375" customWidth="1"/>
+    <col min="22" max="22" width="24.44140625" customWidth="1"/>
+    <col min="23" max="23" width="20.5546875" customWidth="1"/>
+    <col min="24" max="24" width="23.5546875" customWidth="1"/>
+    <col min="25" max="25" width="10.88671875" customWidth="1"/>
+    <col min="26" max="26" width="9.88671875" customWidth="1"/>
+    <col min="27" max="28" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -881,7 +883,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -915,7 +917,7 @@
       <c r="N2" t="s">
         <v>24</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="P2" t="s">
@@ -946,7 +948,7 @@
         <v>43171.312465277777</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -993,7 +995,7 @@
         <v>29</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="S3" s="5" t="s">
         <v>69</v>
@@ -1002,7 +1004,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>93</v>
@@ -1017,7 +1019,7 @@
         <v>43380.740092592598</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1043,10 +1045,13 @@
       <c r="L4" t="s">
         <v>31</v>
       </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
       <c r="N4" t="s">
         <v>24</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="9" t="s">
         <v>33</v>
       </c>
       <c r="P4" t="s">
@@ -1077,7 +1082,7 @@
         <v>43465.51871527778</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1105,10 +1110,13 @@
       <c r="L5" t="s">
         <v>35</v>
       </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
       <c r="N5" t="s">
         <v>24</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="9" t="s">
         <v>22</v>
       </c>
       <c r="P5" t="s">
@@ -1136,7 +1144,7 @@
         <v>43168.402638888889</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1163,11 +1171,13 @@
       <c r="L6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="5"/>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
       <c r="N6" t="s">
         <v>28</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="10" t="s">
         <v>37</v>
       </c>
       <c r="P6" s="5" t="s">
@@ -1186,7 +1196,7 @@
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
       <c r="W6" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="X6" s="5"/>
       <c r="Y6" s="5">
@@ -1199,7 +1209,7 @@
         <v>43398.439317129632</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1233,7 +1243,7 @@
       <c r="N7" t="s">
         <v>24</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="9" t="s">
         <v>22</v>
       </c>
       <c r="P7" t="s">
@@ -1264,7 +1274,7 @@
         <v>43194.333125000005</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1290,10 +1300,13 @@
       <c r="L8" t="s">
         <v>41</v>
       </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
       <c r="N8" t="s">
         <v>24</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" s="9" t="s">
         <v>43</v>
       </c>
       <c r="P8" t="s">
@@ -1315,7 +1328,7 @@
         <v>45</v>
       </c>
       <c r="X8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y8">
         <v>2500</v>
@@ -1327,7 +1340,7 @@
         <v>43245.047384259255</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1353,10 +1366,13 @@
       <c r="L9" t="s">
         <v>46</v>
       </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
       <c r="N9" t="s">
         <v>24</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="9" t="s">
         <v>48</v>
       </c>
       <c r="P9" t="s">
@@ -1369,7 +1385,7 @@
         <v>84</v>
       </c>
       <c r="X9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y9">
         <v>90</v>
@@ -1381,7 +1397,7 @@
         <v>43504.835416666661</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1409,9 +1425,13 @@
       <c r="L10" t="s">
         <v>49</v>
       </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
       <c r="N10" t="s">
         <v>24</v>
       </c>
+      <c r="O10" s="9"/>
       <c r="R10" t="s">
         <v>22</v>
       </c>
@@ -1434,7 +1454,7 @@
         <v>43398.182013888887</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1468,6 +1488,7 @@
       <c r="N11" t="s">
         <v>24</v>
       </c>
+      <c r="O11" s="9"/>
       <c r="S11">
         <v>0</v>
       </c>
@@ -1487,7 +1508,7 @@
         <v>43176.705578703702</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1521,6 +1542,7 @@
       <c r="N12" t="s">
         <v>24</v>
       </c>
+      <c r="O12" s="9"/>
       <c r="R12">
         <v>0</v>
       </c>
@@ -1537,7 +1559,7 @@
         <v>43514.725081018521</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1566,11 +1588,13 @@
       <c r="L13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="M13" s="5"/>
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
       <c r="N13" t="s">
         <v>28</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="O13" s="10" t="s">
         <v>54</v>
       </c>
       <c r="P13" s="5" t="s">
@@ -1589,10 +1613,10 @@
       <c r="U13" s="5"/>
       <c r="V13" s="5"/>
       <c r="W13" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="X13" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Y13" s="5">
         <v>262</v>
@@ -1604,7 +1628,7 @@
         <v>43245.483865740738</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1632,10 +1656,13 @@
       <c r="L14" t="s">
         <v>56</v>
       </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
       <c r="N14" t="s">
         <v>24</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O14" s="9" t="s">
         <v>22</v>
       </c>
       <c r="P14" t="s">
@@ -1666,7 +1693,7 @@
         <v>43434.499907407408</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1693,11 +1720,13 @@
       <c r="L15" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M15" s="5"/>
+      <c r="M15" s="5">
+        <v>0</v>
+      </c>
       <c r="N15" t="s">
         <v>28</v>
       </c>
-      <c r="O15" s="5" t="s">
+      <c r="O15" s="10" t="s">
         <v>59</v>
       </c>
       <c r="P15" s="5" t="s">
@@ -1718,7 +1747,7 @@
       <c r="U15" s="5"/>
       <c r="V15" s="5"/>
       <c r="W15" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="X15" s="5"/>
       <c r="Y15" s="5">
@@ -1731,7 +1760,7 @@
         <v>43371.129965277774</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1765,7 +1794,7 @@
       <c r="N16" t="s">
         <v>24</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O16" s="9" t="s">
         <v>22</v>
       </c>
       <c r="P16" t="s">
@@ -1796,7 +1825,7 @@
         <v>43307.427557870375</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1822,10 +1851,13 @@
       <c r="L17" t="s">
         <v>61</v>
       </c>
+      <c r="M17" s="5">
+        <v>0</v>
+      </c>
       <c r="N17" t="s">
         <v>24</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O17" s="9" t="s">
         <v>62</v>
       </c>
       <c r="P17" t="s">
@@ -1844,7 +1876,7 @@
         <v>43171.089282407404</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1873,11 +1905,13 @@
       <c r="L18" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="M18" s="5"/>
+      <c r="M18" s="5">
+        <v>0</v>
+      </c>
       <c r="N18" t="s">
         <v>28</v>
       </c>
-      <c r="O18" s="5" t="s">
+      <c r="O18" s="10" t="s">
         <v>64</v>
       </c>
       <c r="P18" s="5" t="s">
@@ -1888,16 +1922,16 @@
       </c>
       <c r="R18" s="5"/>
       <c r="S18" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
       <c r="W18" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="X18" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y18" s="5">
         <v>130</v>
@@ -1909,7 +1943,7 @@
         <v>43333.056828703702</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1928,9 +1962,13 @@
       <c r="L19" t="s">
         <v>65</v>
       </c>
+      <c r="M19" s="5">
+        <v>0</v>
+      </c>
       <c r="N19" t="s">
         <v>24</v>
       </c>
+      <c r="O19" s="9"/>
       <c r="S19">
         <v>0</v>
       </c>
@@ -1950,7 +1988,7 @@
         <v>43471.621319444443</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1975,6 +2013,7 @@
       <c r="N20" t="s">
         <v>24</v>
       </c>
+      <c r="O20" s="9"/>
       <c r="W20" t="s">
         <v>25</v>
       </c>
@@ -1988,7 +2027,7 @@
         <v>43198.034942129627</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2022,6 +2061,7 @@
       <c r="N21" t="s">
         <v>24</v>
       </c>
+      <c r="O21" s="9"/>
       <c r="R21" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Added new transaction types in import.sql
</commit_message>
<xml_diff>
--- a/mock_data/20_radku_testovacich_transakci.xlsx
+++ b/mock_data/20_radku_testovacich_transakci.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\moria\mock_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58E9F43-2DAE-42C9-A9E3-55BF312B405F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D9B1A0-382F-4151-9F5F-E2F7395CC0B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="554" xr2:uid="{AC6126E9-B026-468E-A5ED-F833BADB1704}"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="20_radku_testovacich_transakci" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="109">
   <si>
     <t>id</t>
   </si>
@@ -117,9 +117,6 @@
     <t>2018-10-06 19:55:20</t>
   </si>
   <si>
-    <t>INGOING</t>
-  </si>
-  <si>
     <t>00000865</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>0200</t>
   </si>
   <si>
-    <t>OTHER</t>
-  </si>
-  <si>
     <t>2019-02-07 09:58:12</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>2018-03-16 15:58:26</t>
   </si>
   <si>
-    <t>0100</t>
-  </si>
-  <si>
     <t>2019-02-15 21:43:19</t>
   </si>
   <si>
@@ -219,9 +210,6 @@
     <t>2018-03-11 06:42:10</t>
   </si>
   <si>
-    <t>254017692190</t>
-  </si>
-  <si>
     <t>2018-08-20 18:38:38</t>
   </si>
   <si>
@@ -276,9 +264,6 @@
     <t>Sportisimo</t>
   </si>
   <si>
-    <t>Alza</t>
-  </si>
-  <si>
     <t>Steam Store</t>
   </si>
   <si>
@@ -346,6 +331,33 @@
   </si>
   <si>
     <t>Im Lovin It</t>
+  </si>
+  <si>
+    <t>CASH</t>
+  </si>
+  <si>
+    <t>vyber z bankomatu</t>
+  </si>
+  <si>
+    <t>CSOB</t>
+  </si>
+  <si>
+    <t>INCOMING</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>MORTGAGE</t>
+  </si>
+  <si>
+    <t>Splatka hypoteky</t>
+  </si>
+  <si>
+    <t>00000001</t>
+  </si>
+  <si>
+    <t>Hypotecni banka</t>
   </si>
 </sst>
 </file>
@@ -400,7 +412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -416,6 +428,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -766,25 +781,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43CA8FA-B653-44BA-B2F7-6BE6088458A7}">
-  <dimension ref="A1:AA21"/>
+  <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
     <col min="3" max="3" width="18.44140625" customWidth="1"/>
     <col min="4" max="4" width="6.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" customWidth="1"/>
-    <col min="8" max="11" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
     <col min="15" max="15" width="22.5546875" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
     <col min="17" max="17" width="15.44140625" customWidth="1"/>
@@ -826,19 +844,19 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="L1" t="s">
         <v>8</v>
       </c>
       <c r="M1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="N1" t="s">
         <v>9</v>
@@ -862,10 +880,10 @@
         <v>15</v>
       </c>
       <c r="U1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="V1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="W1" t="s">
         <v>16</v>
@@ -897,7 +915,7 @@
         <v>3560</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
         <v>22</v>
@@ -959,10 +977,10 @@
         <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F3" s="5">
         <v>0</v>
@@ -980,37 +998,37 @@
         <v>27</v>
       </c>
       <c r="M3" s="5">
-        <v>11</v>
-      </c>
-      <c r="N3" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="O3" s="8">
         <v>654651579612</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="Y3" s="5">
-        <v>15325</v>
+        <v>17325</v>
       </c>
       <c r="Z3" s="5" t="s">
         <v>26</v>
@@ -1043,7 +1061,7 @@
         <v>20190125</v>
       </c>
       <c r="L4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -1052,25 +1070,28 @@
         <v>24</v>
       </c>
       <c r="O4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" t="s">
         <v>33</v>
       </c>
-      <c r="P4" t="s">
-        <v>34</v>
-      </c>
       <c r="Q4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4" t="s">
-        <v>73</v>
+        <v>69</v>
+      </c>
+      <c r="W4" t="s">
+        <v>98</v>
       </c>
       <c r="X4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="Y4">
         <v>500</v>
@@ -1096,7 +1117,7 @@
         <v>3181</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
@@ -1108,7 +1129,7 @@
         <v>22</v>
       </c>
       <c r="L5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -1169,34 +1190,34 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="O6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="5">
-        <v>0</v>
-      </c>
-      <c r="N6" t="s">
-        <v>28</v>
-      </c>
-      <c r="O6" s="10" t="s">
+      <c r="P6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="P6" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="Q6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R6" s="5">
         <v>0</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
       <c r="W6" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="X6" s="5"/>
       <c r="Y6" s="5">
@@ -1216,14 +1237,12 @@
       <c r="B7">
         <v>6666</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>6821</v>
       </c>
       <c r="E7" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
@@ -1235,22 +1254,22 @@
         <v>22</v>
       </c>
       <c r="L7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M7">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="N7" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="P7" t="s">
-        <v>22</v>
+      <c r="O7" s="11">
+        <v>785845484688</v>
+      </c>
+      <c r="P7" s="4">
+        <v>1500</v>
       </c>
       <c r="Q7" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="R7" t="s">
         <v>22</v>
@@ -1262,7 +1281,10 @@
         <v>22</v>
       </c>
       <c r="W7" t="s">
-        <v>25</v>
+        <v>105</v>
+      </c>
+      <c r="X7" t="s">
+        <v>106</v>
       </c>
       <c r="Y7">
         <v>4099</v>
@@ -1298,7 +1320,7 @@
         <v>927335598</v>
       </c>
       <c r="L8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1307,13 +1329,13 @@
         <v>24</v>
       </c>
       <c r="O8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P8" t="s">
         <v>43</v>
       </c>
-      <c r="P8" t="s">
-        <v>44</v>
-      </c>
       <c r="Q8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R8">
         <v>0</v>
@@ -1322,13 +1344,13 @@
         <v>0</v>
       </c>
       <c r="T8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="W8" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="X8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="Y8">
         <v>2500</v>
@@ -1364,7 +1386,7 @@
         <v>4848218390</v>
       </c>
       <c r="L9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1373,19 +1395,22 @@
         <v>24</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="T9" t="s">
-        <v>84</v>
+        <v>79</v>
+      </c>
+      <c r="W9" t="s">
+        <v>98</v>
       </c>
       <c r="X9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="Y9">
         <v>90</v>
@@ -1405,13 +1430,13 @@
         <v>6666</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1">
         <v>7277</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
@@ -1423,7 +1448,7 @@
         <v>22</v>
       </c>
       <c r="L10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1462,13 +1487,13 @@
         <v>6666</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="4">
         <v>5968</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1480,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M11">
         <v>118</v>
@@ -1516,13 +1541,13 @@
         <v>6666</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="4">
         <v>4899</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1534,7 +1559,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="M12">
         <v>118</v>
@@ -1550,7 +1575,7 @@
         <v>25</v>
       </c>
       <c r="Y12">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="Z12" t="s">
         <v>26</v>
@@ -1586,37 +1611,37 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M13" s="5">
         <v>0</v>
       </c>
-      <c r="N13" t="s">
-        <v>28</v>
+      <c r="N13" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="O13" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R13" s="5">
         <v>0</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
       <c r="V13" s="5"/>
       <c r="W13" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="X13" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="Y13" s="5">
         <v>262</v>
@@ -1636,13 +1661,13 @@
         <v>6666</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1">
         <v>3560</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F14" t="s">
         <v>22</v>
@@ -1654,7 +1679,7 @@
         <v>22</v>
       </c>
       <c r="L14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1684,7 +1709,7 @@
         <v>25</v>
       </c>
       <c r="Y14">
-        <v>1892</v>
+        <v>2392</v>
       </c>
       <c r="Z14" t="s">
         <v>26</v>
@@ -1718,22 +1743,22 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M15" s="5">
         <v>0</v>
       </c>
-      <c r="N15" t="s">
-        <v>28</v>
+      <c r="N15" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="O15" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="P15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q15" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="Q15" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="R15" s="5">
         <v>0</v>
@@ -1747,7 +1772,7 @@
       <c r="U15" s="5"/>
       <c r="V15" s="5"/>
       <c r="W15" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="X15" s="5"/>
       <c r="Y15" s="5">
@@ -1774,7 +1799,7 @@
         <v>3110</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F16" t="s">
         <v>22</v>
@@ -1786,7 +1811,7 @@
         <v>22</v>
       </c>
       <c r="L16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M16">
         <v>119</v>
@@ -1804,7 +1829,7 @@
         <v>22</v>
       </c>
       <c r="R16" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="S16" t="s">
         <v>22</v>
@@ -1832,42 +1857,33 @@
       <c r="B17">
         <v>6666</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D17" s="1" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="E17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>5135551790</v>
+        <v>102</v>
       </c>
       <c r="L17" t="s">
-        <v>61</v>
-      </c>
-      <c r="M17" s="5">
+        <v>58</v>
+      </c>
+      <c r="M17">
         <v>0</v>
       </c>
       <c r="N17" t="s">
         <v>24</v>
       </c>
-      <c r="O17" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="P17" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>32</v>
+      <c r="O17" s="9"/>
+      <c r="W17" t="s">
+        <v>100</v>
+      </c>
+      <c r="X17" t="s">
+        <v>101</v>
       </c>
       <c r="Y17">
-        <v>515</v>
+        <v>5000</v>
       </c>
       <c r="Z17" t="s">
         <v>26</v>
@@ -1903,35 +1919,35 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M18" s="5">
         <v>0</v>
       </c>
-      <c r="N18" t="s">
-        <v>28</v>
+      <c r="N18" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="O18" s="10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R18" s="5"/>
       <c r="S18" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
       <c r="W18" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="X18" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="Y18" s="5">
         <v>130</v>
@@ -1954,15 +1970,15 @@
         <v>21</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L19" t="s">
-        <v>65</v>
-      </c>
-      <c r="M19" s="5">
+        <v>61</v>
+      </c>
+      <c r="M19">
         <v>0</v>
       </c>
       <c r="N19" t="s">
@@ -1996,16 +2012,16 @@
         <v>6666</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="L20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="M20">
         <v>124</v>
@@ -2035,13 +2051,13 @@
         <v>6666</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="1">
         <v>4449</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F21" t="s">
         <v>22</v>
@@ -2053,7 +2069,7 @@
         <v>22</v>
       </c>
       <c r="L21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="M21">
         <v>115</v>
@@ -2082,6 +2098,22 @@
       </c>
       <c r="AA21" s="3">
         <v>43255.333449074074</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="Y26">
+        <f>SUM(Y2:Y21)</f>
+        <v>42000</v>
+      </c>
+      <c r="Z26">
+        <f>SUM(Y3+Y6+Y13+Y15+Y18)</f>
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="Z27">
+        <f>Y26-Z26</f>
+        <v>20000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new mock ruleset and payment to be tested, fixed typos, deleted Item.java
</commit_message>
<xml_diff>
--- a/mock_data/20_radku_testovacich_transakci.xlsx
+++ b/mock_data/20_radku_testovacich_transakci.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\moria\mock_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D9B1A0-382F-4151-9F5F-E2F7395CC0B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB8565D-1E79-4D34-96D3-98E75EA39041}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="554" xr2:uid="{AC6126E9-B026-468E-A5ED-F833BADB1704}"/>
   </bookViews>
@@ -784,7 +784,7 @@
   <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Hiding percentage if sector is too small, mock data source fix
</commit_message>
<xml_diff>
--- a/mock_data/20_radku_testovacich_transakci.xlsx
+++ b/mock_data/20_radku_testovacich_transakci.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\moria\mock_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB8565D-1E79-4D34-96D3-98E75EA39041}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67842060-61CE-4C36-AC1F-FFA09D8DAA05}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="554" xr2:uid="{AC6126E9-B026-468E-A5ED-F833BADB1704}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="108">
   <si>
     <t>id</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>2018-05-24 01:31:58</t>
-  </si>
-  <si>
-    <t>191816107239</t>
   </si>
   <si>
     <t>0800</t>
@@ -412,7 +409,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -429,6 +426,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -783,42 +783,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43CA8FA-B653-44BA-B2F7-6BE6088458A7}">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="6.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="22.5546875" customWidth="1"/>
+    <col min="15" max="15" width="23.5703125" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="15.44140625" customWidth="1"/>
-    <col min="18" max="18" width="18.88671875" customWidth="1"/>
-    <col min="19" max="19" width="22.109375" customWidth="1"/>
-    <col min="20" max="20" width="24.44140625" customWidth="1"/>
-    <col min="21" max="21" width="22.109375" customWidth="1"/>
-    <col min="22" max="22" width="24.44140625" customWidth="1"/>
-    <col min="23" max="23" width="20.5546875" customWidth="1"/>
-    <col min="24" max="24" width="23.5546875" customWidth="1"/>
-    <col min="25" max="25" width="10.88671875" customWidth="1"/>
-    <col min="26" max="26" width="9.88671875" customWidth="1"/>
-    <col min="27" max="28" width="19.44140625" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" customWidth="1"/>
+    <col min="20" max="20" width="24.42578125" customWidth="1"/>
+    <col min="21" max="21" width="22.140625" customWidth="1"/>
+    <col min="22" max="22" width="24.42578125" customWidth="1"/>
+    <col min="23" max="23" width="20.5703125" customWidth="1"/>
+    <col min="24" max="24" width="23.5703125" customWidth="1"/>
+    <col min="25" max="25" width="10.85546875" customWidth="1"/>
+    <col min="26" max="26" width="9.85546875" customWidth="1"/>
+    <col min="27" max="28" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -844,19 +844,19 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>81</v>
-      </c>
-      <c r="K1" t="s">
-        <v>82</v>
       </c>
       <c r="L1" t="s">
         <v>8</v>
       </c>
       <c r="M1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N1" t="s">
         <v>9</v>
@@ -880,10 +880,10 @@
         <v>15</v>
       </c>
       <c r="U1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" t="s">
         <v>84</v>
-      </c>
-      <c r="V1" t="s">
-        <v>85</v>
       </c>
       <c r="W1" t="s">
         <v>16</v>
@@ -901,7 +901,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -915,7 +915,7 @@
         <v>3560</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
         <v>22</v>
@@ -938,10 +938,10 @@
       <c r="O2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="P2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="R2" t="s">
@@ -966,7 +966,7 @@
         <v>43171.312465277777</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -977,10 +977,10 @@
         <v>21</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="5">
         <v>0</v>
@@ -1001,31 +1001,31 @@
         <v>0</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O3" s="8">
         <v>654651579612</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="7" t="s">
         <v>28</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Y3" s="5">
         <v>17325</v>
@@ -1037,7 +1037,7 @@
         <v>43380.740092592598</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1072,26 +1072,26 @@
       <c r="O4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="R4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="W4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Y4">
         <v>500</v>
@@ -1103,7 +1103,7 @@
         <v>43465.51871527778</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>3181</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
@@ -1140,10 +1140,10 @@
       <c r="O5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="P5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="P5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="R5" t="s">
@@ -1165,7 +1165,7 @@
         <v>43168.402638888889</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1196,28 +1196,28 @@
         <v>0</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="Q6" s="5" t="s">
+      <c r="Q6" s="7" t="s">
         <v>31</v>
       </c>
       <c r="R6" s="5">
         <v>0</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
       <c r="W6" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X6" s="5"/>
       <c r="Y6" s="5">
@@ -1230,7 +1230,7 @@
         <v>43398.439317129632</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>6821</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
@@ -1257,7 +1257,7 @@
         <v>39</v>
       </c>
       <c r="M7">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="N7" t="s">
         <v>24</v>
@@ -1265,11 +1265,11 @@
       <c r="O7" s="11">
         <v>785845484688</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="12">
         <v>1500</v>
       </c>
-      <c r="Q7" t="s">
-        <v>107</v>
+      <c r="Q7" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="R7" t="s">
         <v>22</v>
@@ -1281,10 +1281,10 @@
         <v>22</v>
       </c>
       <c r="W7" t="s">
+        <v>104</v>
+      </c>
+      <c r="X7" t="s">
         <v>105</v>
-      </c>
-      <c r="X7" t="s">
-        <v>106</v>
       </c>
       <c r="Y7">
         <v>4099</v>
@@ -1296,7 +1296,7 @@
         <v>43194.333125000005</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1331,10 +1331,10 @@
       <c r="O8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" s="1" t="s">
         <v>41</v>
       </c>
       <c r="R8">
@@ -1344,13 +1344,13 @@
         <v>0</v>
       </c>
       <c r="T8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Y8">
         <v>2500</v>
@@ -1362,7 +1362,7 @@
         <v>43245.047384259255</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1397,20 +1397,20 @@
       <c r="O9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="1" t="s">
         <v>45</v>
       </c>
       <c r="T9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Y9">
         <v>90</v>
@@ -1422,7 +1422,7 @@
         <v>43504.835416666661</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>7277</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
@@ -1457,6 +1457,8 @@
         <v>24</v>
       </c>
       <c r="O10" s="9"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
       <c r="R10" t="s">
         <v>22</v>
       </c>
@@ -1479,7 +1481,7 @@
         <v>43398.182013888887</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1493,7 +1495,7 @@
         <v>5968</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1514,6 +1516,8 @@
         <v>24</v>
       </c>
       <c r="O11" s="9"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
       <c r="S11">
         <v>0</v>
       </c>
@@ -1533,7 +1537,7 @@
         <v>43176.705578703702</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1547,7 +1551,7 @@
         <v>4899</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1568,6 +1572,8 @@
         <v>24</v>
       </c>
       <c r="O12" s="9"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
       <c r="R12">
         <v>0</v>
       </c>
@@ -1584,7 +1590,7 @@
         <v>43514.725081018521</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1617,31 +1623,31 @@
         <v>0</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="O13" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="O13" s="8">
+        <v>191816107239</v>
+      </c>
+      <c r="P13" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="P13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q13" s="5" t="s">
+      <c r="Q13" s="7" t="s">
         <v>31</v>
       </c>
       <c r="R13" s="5">
         <v>0</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
       <c r="V13" s="5"/>
       <c r="W13" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X13" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Y13" s="5">
         <v>262</v>
@@ -1653,7 +1659,7 @@
         <v>43245.483865740738</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1667,7 +1673,7 @@
         <v>3560</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F14" t="s">
         <v>22</v>
@@ -1679,7 +1685,7 @@
         <v>22</v>
       </c>
       <c r="L14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1690,10 +1696,10 @@
       <c r="O14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="P14" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q14" t="s">
+      <c r="P14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="R14" t="s">
@@ -1718,7 +1724,7 @@
         <v>43434.499907407408</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1743,22 +1749,22 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M15" s="5">
+        <v>0</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q15" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="M15" s="5">
-        <v>0</v>
-      </c>
-      <c r="N15" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="O15" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="P15" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q15" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="R15" s="5">
         <v>0</v>
@@ -1772,7 +1778,7 @@
       <c r="U15" s="5"/>
       <c r="V15" s="5"/>
       <c r="W15" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X15" s="5"/>
       <c r="Y15" s="5">
@@ -1785,7 +1791,7 @@
         <v>43371.129965277774</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1799,7 +1805,7 @@
         <v>3110</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" t="s">
         <v>22</v>
@@ -1811,7 +1817,7 @@
         <v>22</v>
       </c>
       <c r="L16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M16">
         <v>119</v>
@@ -1822,14 +1828,14 @@
       <c r="O16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="P16" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q16" t="s">
+      <c r="P16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="R16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S16" t="s">
         <v>22</v>
@@ -1850,7 +1856,7 @@
         <v>43307.427557870375</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1861,13 +1867,13 @@
         <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -1876,11 +1882,13 @@
         <v>24</v>
       </c>
       <c r="O17" s="9"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
       <c r="W17" t="s">
+        <v>99</v>
+      </c>
+      <c r="X17" t="s">
         <v>100</v>
-      </c>
-      <c r="X17" t="s">
-        <v>101</v>
       </c>
       <c r="Y17">
         <v>5000</v>
@@ -1892,7 +1900,7 @@
         <v>43171.089282407404</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1919,35 +1927,35 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="M18" s="5">
+        <v>0</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O18" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="M18" s="5">
-        <v>0</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="O18" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="P18" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q18" s="5" t="s">
+      <c r="P18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q18" s="7" t="s">
         <v>31</v>
       </c>
       <c r="R18" s="5"/>
       <c r="S18" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
       <c r="W18" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X18" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y18" s="5">
         <v>130</v>
@@ -1959,7 +1967,7 @@
         <v>43333.056828703702</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1970,13 +1978,13 @@
         <v>21</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -1985,6 +1993,8 @@
         <v>24</v>
       </c>
       <c r="O19" s="9"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
       <c r="S19">
         <v>0</v>
       </c>
@@ -2004,7 +2014,7 @@
         <v>43471.621319444443</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2015,13 +2025,13 @@
         <v>38</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M20">
         <v>124</v>
@@ -2030,6 +2040,8 @@
         <v>24</v>
       </c>
       <c r="O20" s="9"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
       <c r="W20" t="s">
         <v>25</v>
       </c>
@@ -2043,7 +2055,7 @@
         <v>43198.034942129627</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2057,7 +2069,7 @@
         <v>4449</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F21" t="s">
         <v>22</v>
@@ -2069,7 +2081,7 @@
         <v>22</v>
       </c>
       <c r="L21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M21">
         <v>115</v>
@@ -2078,6 +2090,8 @@
         <v>24</v>
       </c>
       <c r="O21" s="9"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
       <c r="R21" t="s">
         <v>22</v>
       </c>
@@ -2100,7 +2114,7 @@
         <v>43255.333449074074</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="Y26">
         <f>SUM(Y2:Y21)</f>
         <v>42000</v>
@@ -2110,7 +2124,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="Z27">
         <f>Y26-Z26</f>
         <v>20000</v>

</xml_diff>

<commit_message>
Improved categorization test, ordered parametres in testUtils to match Model and import.sql
</commit_message>
<xml_diff>
--- a/mock_data/20_radku_testovacich_transakci.xlsx
+++ b/mock_data/20_radku_testovacich_transakci.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\moria\mock_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67842060-61CE-4C36-AC1F-FFA09D8DAA05}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F2329C-B8BF-450F-B13D-46596DB0E3AE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="554" xr2:uid="{AC6126E9-B026-468E-A5ED-F833BADB1704}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="554" xr2:uid="{AC6126E9-B026-468E-A5ED-F833BADB1704}"/>
   </bookViews>
   <sheets>
     <sheet name="20_radku_testovacich_transakci" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="113">
   <si>
     <t>id</t>
   </si>
@@ -355,6 +355,21 @@
   </si>
   <si>
     <t>Hypotecni banka</t>
+  </si>
+  <si>
+    <t>cílová kategorie</t>
+  </si>
+  <si>
+    <t>už zařazeno</t>
+  </si>
+  <si>
+    <t>zařadí algoritmus</t>
+  </si>
+  <si>
+    <t>příjmy</t>
+  </si>
+  <si>
+    <t>výdaje</t>
   </si>
 </sst>
 </file>
@@ -365,7 +380,7 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,8 +397,24 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,8 +426,23 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -404,12 +450,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -431,10 +550,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
     <cellStyle name="Správně" xfId="1" builtinId="26"/>
+    <cellStyle name="Špatně" xfId="2" builtinId="27"/>
+    <cellStyle name="Zvýraznění 1" xfId="3" builtinId="29"/>
+    <cellStyle name="Zvýraznění 6" xfId="4" builtinId="49"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -781,170 +914,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43CA8FA-B653-44BA-B2F7-6BE6088458A7}">
-  <dimension ref="A1:AA27"/>
+  <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB24" sqref="AB24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
-    <col min="12" max="12" width="20" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" customWidth="1"/>
-    <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="15" max="15" width="23.5703125" customWidth="1"/>
-    <col min="16" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" customWidth="1"/>
-    <col min="18" max="18" width="18.85546875" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" customWidth="1"/>
-    <col min="20" max="20" width="24.42578125" customWidth="1"/>
-    <col min="21" max="21" width="22.140625" customWidth="1"/>
-    <col min="22" max="22" width="24.42578125" customWidth="1"/>
-    <col min="23" max="23" width="20.5703125" customWidth="1"/>
-    <col min="24" max="24" width="23.5703125" customWidth="1"/>
-    <col min="25" max="25" width="10.85546875" customWidth="1"/>
-    <col min="26" max="26" width="9.85546875" customWidth="1"/>
-    <col min="27" max="28" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
+    <col min="16" max="16" width="23.5703125" customWidth="1"/>
+    <col min="17" max="17" width="14" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" customWidth="1"/>
+    <col min="19" max="19" width="18.85546875" customWidth="1"/>
+    <col min="20" max="20" width="22.140625" customWidth="1"/>
+    <col min="21" max="21" width="24.42578125" customWidth="1"/>
+    <col min="22" max="22" width="22.140625" customWidth="1"/>
+    <col min="23" max="23" width="24.42578125" customWidth="1"/>
+    <col min="24" max="24" width="20.5703125" customWidth="1"/>
+    <col min="25" max="25" width="23.5703125" customWidth="1"/>
+    <col min="26" max="26" width="10.85546875" customWidth="1"/>
+    <col min="27" max="27" width="9.85546875" customWidth="1"/>
+    <col min="28" max="28" width="21.140625" customWidth="1"/>
+    <col min="29" max="29" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>79</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>80</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>81</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>82</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>10</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>83</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>84</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>16</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>111</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>6666</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>3560</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>63</v>
       </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
       <c r="G2" t="s">
         <v>22</v>
       </c>
       <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>111</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="S2" t="s">
@@ -953,756 +1092,792 @@
       <c r="T2" t="s">
         <v>22</v>
       </c>
-      <c r="W2" t="s">
+      <c r="U2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X2" t="s">
         <v>25</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>1521</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>26</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AB2" s="3">
         <v>43171.312465277777</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>11</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>6666</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
       <c r="G3" s="5">
         <v>0</v>
       </c>
       <c r="H3" s="5">
         <v>0</v>
       </c>
-      <c r="I3" s="5"/>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="5"/>
+      <c r="M3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="5">
-        <v>0</v>
-      </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="O3" s="8">
+      <c r="P3" s="8">
         <v>654651579612</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="R3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
-      <c r="W3" s="5" t="s">
+      <c r="W3" s="5"/>
+      <c r="X3" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="Y3" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="Y3" s="5">
+      <c r="Z3" s="5">
         <v>17325</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="AA3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AA3" s="6">
-        <v>43380.740092592598</v>
+      <c r="AB3" s="6">
+        <v>43380.74009259259</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>6666</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>20190125</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>30</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>89</v>
       </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4" t="s">
         <v>68</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>97</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>88</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>500</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>26</v>
       </c>
-      <c r="AA4" s="3">
+      <c r="AB4" s="3">
         <v>43465.51871527778</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>6666</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>3181</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>75</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
       <c r="G5" t="s">
         <v>22</v>
       </c>
       <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="L5" t="s">
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s">
         <v>34</v>
       </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
         <v>24</v>
       </c>
-      <c r="O5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="9" t="s">
         <v>22</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="S5" t="s">
         <v>22</v>
       </c>
-      <c r="W5" t="s">
+      <c r="T5" t="s">
+        <v>22</v>
+      </c>
+      <c r="X5" t="s">
         <v>25</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>899</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>26</v>
       </c>
-      <c r="AA5" s="3">
+      <c r="AB5" s="3">
         <v>43168.402638888889</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>6666</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5">
-        <v>0</v>
-      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="5"/>
       <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
         <v>5387662130</v>
       </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5"/>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="5"/>
+      <c r="M6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="5">
-        <v>0</v>
-      </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="P6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="Q6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="R6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="R6" s="5">
-        <v>0</v>
-      </c>
-      <c r="S6" s="5" t="s">
+      <c r="S6" s="5">
+        <v>0</v>
+      </c>
+      <c r="T6" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="T6" s="5"/>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
-      <c r="W6" s="5" t="s">
+      <c r="W6" s="5"/>
+      <c r="X6" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5">
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5">
         <v>4200</v>
       </c>
-      <c r="Z6" s="5" t="s">
+      <c r="AA6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AA6" s="6">
+      <c r="AB6" s="6">
         <v>43398.439317129632</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>128</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>6666</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
         <v>6821</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>107</v>
       </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
       <c r="G7" t="s">
         <v>22</v>
       </c>
       <c r="H7" t="s">
         <v>22</v>
       </c>
-      <c r="L7" t="s">
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" t="s">
         <v>39</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="11">
+      <c r="P7" s="11">
         <v>785845484688</v>
       </c>
-      <c r="P7" s="12">
+      <c r="Q7" s="12">
         <v>1500</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="R7" t="s">
-        <v>22</v>
-      </c>
       <c r="S7" t="s">
         <v>22</v>
       </c>
       <c r="T7" t="s">
         <v>22</v>
       </c>
-      <c r="W7" t="s">
+      <c r="U7" t="s">
+        <v>22</v>
+      </c>
+      <c r="X7" t="s">
         <v>104</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>105</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>4099</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>26</v>
       </c>
-      <c r="AA7" s="3">
+      <c r="AB7" s="3">
         <v>43194.333125000005</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>6666</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8">
         <v>4482</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
       <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>927335598</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>40</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="P8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
       <c r="S8">
         <v>0</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8" t="s">
         <v>69</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>97</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>92</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>2500</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>26</v>
       </c>
-      <c r="AA8" s="3">
+      <c r="AB8" s="3">
         <v>43245.047384259255</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>6666</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9">
         <v>3347</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
       <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>4848218390</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>44</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
         <v>24</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="P9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>78</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>97</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>93</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>90</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>26</v>
       </c>
-      <c r="AA9" s="3">
+      <c r="AB9" s="3">
         <v>43504.835416666661</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>6666</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>7277</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>70</v>
       </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
       <c r="G10" t="s">
         <v>22</v>
       </c>
       <c r="H10" t="s">
         <v>22</v>
       </c>
-      <c r="L10" t="s">
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" t="s">
         <v>47</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" t="s">
         <v>24</v>
       </c>
-      <c r="O10" s="9"/>
-      <c r="P10" s="1"/>
+      <c r="P10" s="9"/>
       <c r="Q10" s="1"/>
-      <c r="R10" t="s">
-        <v>22</v>
-      </c>
+      <c r="R10" s="1"/>
       <c r="S10" t="s">
         <v>22</v>
       </c>
       <c r="T10" t="s">
         <v>22</v>
       </c>
-      <c r="W10" t="s">
+      <c r="U10" t="s">
+        <v>22</v>
+      </c>
+      <c r="X10" t="s">
         <v>25</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>249</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AA10" t="s">
         <v>26</v>
       </c>
-      <c r="AA10" s="3">
+      <c r="AB10" s="3">
         <v>43398.182013888887</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>118</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>6666</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="4">
         <v>5968</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>72</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="L11" t="s">
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
         <v>48</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>118</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="9"/>
-      <c r="P11" s="1"/>
+      <c r="P11" s="9"/>
       <c r="Q11" s="1"/>
-      <c r="S11">
-        <v>0</v>
-      </c>
+      <c r="R11" s="1"/>
       <c r="T11">
         <v>0</v>
       </c>
-      <c r="W11" t="s">
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="X11" t="s">
         <v>25</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>230</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AA11" t="s">
         <v>26</v>
       </c>
-      <c r="AA11" s="3">
+      <c r="AB11" s="3">
         <v>43176.705578703702</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>118</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>6666</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="4">
         <v>4899</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>73</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="L12" t="s">
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="M12" t="s">
         <v>49</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>118</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="9"/>
-      <c r="P12" s="1"/>
+      <c r="P12" s="9"/>
       <c r="Q12" s="1"/>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="W12" t="s">
+      <c r="R12" s="1"/>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="X12" t="s">
         <v>25</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <v>85</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AA12" t="s">
         <v>26</v>
       </c>
-      <c r="AA12" s="3">
+      <c r="AB12" s="3">
         <v>43514.725081018521</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>17</v>
+      </c>
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>6666</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="D13" s="1"/>
+      <c r="E13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="5">
         <v>6771</v>
       </c>
-      <c r="G13" s="5">
-        <v>0</v>
-      </c>
       <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
         <v>4457394676</v>
       </c>
-      <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="5"/>
+      <c r="M13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="M13" s="5">
-        <v>0</v>
-      </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="5">
+        <v>0</v>
+      </c>
+      <c r="O13" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="O13" s="8">
+      <c r="P13" s="8">
         <v>191816107239</v>
       </c>
-      <c r="P13" s="7" t="s">
+      <c r="Q13" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="Q13" s="7" t="s">
+      <c r="R13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="R13" s="5">
-        <v>0</v>
-      </c>
-      <c r="S13" s="5" t="s">
+      <c r="S13" s="5">
+        <v>0</v>
+      </c>
+      <c r="T13" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="T13" s="5"/>
       <c r="U13" s="5"/>
       <c r="V13" s="5"/>
-      <c r="W13" s="5" t="s">
+      <c r="W13" s="5"/>
+      <c r="X13" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="X13" s="5" t="s">
+      <c r="Y13" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="Y13" s="5">
+      <c r="Z13" s="5">
         <v>262</v>
       </c>
-      <c r="Z13" s="5" t="s">
+      <c r="AA13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AA13" s="6">
+      <c r="AB13" s="6">
         <v>43245.483865740738</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>6666</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>3560</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>63</v>
       </c>
-      <c r="F14" t="s">
-        <v>22</v>
-      </c>
       <c r="G14" t="s">
         <v>22</v>
       </c>
       <c r="H14" t="s">
         <v>22</v>
       </c>
-      <c r="L14" t="s">
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" t="s">
         <v>52</v>
       </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
         <v>24</v>
       </c>
-      <c r="O14" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="P14" s="1" t="s">
+      <c r="P14" s="9" t="s">
         <v>22</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="S14" t="s">
@@ -1711,440 +1886,473 @@
       <c r="T14" t="s">
         <v>22</v>
       </c>
-      <c r="W14" t="s">
+      <c r="U14" t="s">
+        <v>22</v>
+      </c>
+      <c r="X14" t="s">
         <v>25</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <v>2392</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AA14" t="s">
         <v>26</v>
       </c>
-      <c r="AA14" s="3">
+      <c r="AB14" s="3">
         <v>43434.499907407408</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>6666</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5">
-        <v>0</v>
-      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="5"/>
       <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5">
         <v>6484975897</v>
       </c>
-      <c r="H15" s="5">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="5"/>
+      <c r="M15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="M15" s="5">
-        <v>0</v>
-      </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="5">
+        <v>0</v>
+      </c>
+      <c r="O15" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="O15" s="10" t="s">
+      <c r="P15" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="P15" s="7" t="s">
+      <c r="Q15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="Q15" s="7" t="s">
+      <c r="R15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R15" s="5">
-        <v>0</v>
-      </c>
       <c r="S15" s="5">
         <v>0</v>
       </c>
       <c r="T15" s="5">
         <v>0</v>
       </c>
-      <c r="U15" s="5"/>
+      <c r="U15" s="5">
+        <v>0</v>
+      </c>
       <c r="V15" s="5"/>
-      <c r="W15" s="5" t="s">
+      <c r="W15" s="5"/>
+      <c r="X15" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5">
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5">
         <v>83</v>
       </c>
-      <c r="Z15" s="5" t="s">
+      <c r="AA15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AA15" s="6">
+      <c r="AB15" s="6">
         <v>43371.129965277774</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>119</v>
+      </c>
+      <c r="B16">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>6666</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>3110</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>71</v>
       </c>
-      <c r="F16" t="s">
-        <v>22</v>
-      </c>
       <c r="G16" t="s">
         <v>22</v>
       </c>
       <c r="H16" t="s">
         <v>22</v>
       </c>
-      <c r="L16" t="s">
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" t="s">
         <v>56</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>119</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="P16" s="1" t="s">
+      <c r="P16" s="9" t="s">
         <v>22</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S16" t="s">
         <v>91</v>
       </c>
-      <c r="S16" t="s">
-        <v>22</v>
-      </c>
       <c r="T16" t="s">
         <v>22</v>
       </c>
-      <c r="W16" t="s">
+      <c r="U16" t="s">
+        <v>22</v>
+      </c>
+      <c r="X16" t="s">
         <v>25</v>
       </c>
-      <c r="Y16">
+      <c r="Z16">
         <v>157</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AA16" t="s">
         <v>26</v>
       </c>
-      <c r="AA16" s="3">
+      <c r="AB16" s="3">
         <v>43307.427557870375</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>131</v>
+      </c>
+      <c r="B17">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>6666</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>101</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>57</v>
       </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17" t="s">
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
         <v>24</v>
       </c>
-      <c r="O17" s="9"/>
-      <c r="P17" s="1"/>
+      <c r="P17" s="9"/>
       <c r="Q17" s="1"/>
-      <c r="W17" t="s">
+      <c r="R17" s="1"/>
+      <c r="X17" t="s">
         <v>99</v>
       </c>
-      <c r="X17" t="s">
+      <c r="Y17" t="s">
         <v>100</v>
       </c>
-      <c r="Y17">
+      <c r="Z17">
         <v>5000</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AA17" t="s">
         <v>26</v>
       </c>
-      <c r="AA17" s="3">
+      <c r="AB17" s="3">
         <v>43171.089282407404</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>6666</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="5">
+      <c r="D18" s="1"/>
+      <c r="E18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="5">
         <v>3317</v>
       </c>
-      <c r="G18" s="5">
-        <v>0</v>
-      </c>
       <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
         <v>777</v>
       </c>
-      <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="5" t="s">
+      <c r="L18" s="5"/>
+      <c r="M18" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="M18" s="5">
-        <v>0</v>
-      </c>
-      <c r="N18" s="5" t="s">
+      <c r="N18" s="5">
+        <v>0</v>
+      </c>
+      <c r="O18" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="O18" s="10" t="s">
+      <c r="P18" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="P18" s="7" t="s">
+      <c r="Q18" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="Q18" s="7" t="s">
+      <c r="R18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5" t="s">
+      <c r="S18" s="5"/>
+      <c r="T18" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="T18" s="5"/>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
-      <c r="W18" s="5" t="s">
+      <c r="W18" s="5"/>
+      <c r="X18" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="X18" s="5" t="s">
+      <c r="Y18" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="Y18" s="5">
+      <c r="Z18" s="5">
         <v>130</v>
       </c>
-      <c r="Z18" s="5" t="s">
+      <c r="AA18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AA18" s="6">
+      <c r="AB18" s="6">
         <v>43333.056828703702</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>6666</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>76</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>60</v>
       </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19" t="s">
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
         <v>24</v>
       </c>
-      <c r="O19" s="9"/>
-      <c r="P19" s="1"/>
+      <c r="P19" s="9"/>
       <c r="Q19" s="1"/>
-      <c r="S19">
-        <v>0</v>
-      </c>
+      <c r="R19" s="1"/>
       <c r="T19">
         <v>0</v>
       </c>
-      <c r="W19" t="s">
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="X19" t="s">
         <v>25</v>
       </c>
-      <c r="Y19">
+      <c r="Z19">
         <v>1963</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="AA19" t="s">
         <v>26</v>
       </c>
-      <c r="AA19" s="3">
+      <c r="AB19" s="3">
         <v>43471.621319444443</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>124</v>
+      </c>
+      <c r="B20">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>6666</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>86</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>61</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>124</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>24</v>
       </c>
-      <c r="O20" s="9"/>
-      <c r="P20" s="1"/>
+      <c r="P20" s="9"/>
       <c r="Q20" s="1"/>
-      <c r="W20" t="s">
+      <c r="R20" s="1"/>
+      <c r="X20" t="s">
         <v>25</v>
       </c>
-      <c r="Y20">
+      <c r="Z20">
         <v>260</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="AA20" t="s">
         <v>26</v>
       </c>
-      <c r="AA20" s="3">
+      <c r="AB20" s="3">
         <v>43198.034942129627</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>115</v>
+      </c>
+      <c r="B21">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>6666</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>4449</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>74</v>
       </c>
-      <c r="F21" t="s">
-        <v>22</v>
-      </c>
       <c r="G21" t="s">
         <v>22</v>
       </c>
       <c r="H21" t="s">
         <v>22</v>
       </c>
-      <c r="L21" t="s">
+      <c r="I21" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" t="s">
         <v>62</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>115</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>24</v>
       </c>
-      <c r="O21" s="9"/>
-      <c r="P21" s="1"/>
+      <c r="P21" s="9"/>
       <c r="Q21" s="1"/>
-      <c r="R21" t="s">
-        <v>22</v>
-      </c>
+      <c r="R21" s="1"/>
       <c r="S21" t="s">
         <v>22</v>
       </c>
       <c r="T21" t="s">
         <v>22</v>
       </c>
-      <c r="W21" t="s">
+      <c r="U21" t="s">
+        <v>22</v>
+      </c>
+      <c r="X21" t="s">
         <v>25</v>
       </c>
-      <c r="Y21">
+      <c r="Z21">
         <v>55</v>
       </c>
-      <c r="Z21" t="s">
+      <c r="AA21" t="s">
         <v>26</v>
       </c>
-      <c r="AA21" s="3">
+      <c r="AB21" s="3">
         <v>43255.333449074074</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="Y26">
-        <f>SUM(Y2:Y21)</f>
-        <v>42000</v>
-      </c>
-      <c r="Z26">
-        <f>SUM(Y3+Y6+Y13+Y15+Y18)</f>
+    <row r="23" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z24" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA24" s="19">
+        <f>SUM(Z3+Z6+Z13+Z15+Z18)</f>
         <v>22000</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="Z27">
-        <f>Y26-Z26</f>
+    <row r="25" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z25" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA25" s="21">
+        <f>SUM(Z2:Z21)-AA24</f>
         <v>20000</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="N1:N1048576">
+  <conditionalFormatting sqref="O1:O1048576">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="outgoing">
-      <formula>NOT(ISERROR(SEARCH("outgoing",N1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("outgoing",O1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="INGOING">
-      <formula>NOT(ISERROR(SEARCH("INGOING",N1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("INGOING",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="4562356984521568">
-      <formula>NOT(ISERROR(SEARCH("4562356984521568",C1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("4562356984521568",D1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="354265892135264">
-      <formula>NOT(ISERROR(SEARCH("354265892135264",C1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("354265892135264",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed is_category_manually_assigned and parent_id in mock data
</commit_message>
<xml_diff>
--- a/mock_data/20_radku_testovacich_transakci.xlsx
+++ b/mock_data/20_radku_testovacich_transakci.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\moria\mock_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3508A72F-93CB-41BE-A3EF-F8C5BD641A18}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A861A3B-B8FC-4031-A796-C8B7A3576AC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="554" xr2:uid="{AC6126E9-B026-468E-A5ED-F833BADB1704}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="554" xr2:uid="{AC6126E9-B026-468E-A5ED-F833BADB1704}"/>
   </bookViews>
   <sheets>
     <sheet name="20_radku_testovacich_transakci" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="152">
   <si>
     <t>id</t>
   </si>
@@ -713,7 +713,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="6" applyAlignment="1">
@@ -767,29 +767,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -1168,141 +1163,141 @@
   <dimension ref="A1:AE31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="S8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="V11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A9" activeCellId="1" sqref="A22:XFD22 A9:XFD9"/>
+      <selection pane="bottomRight" activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="16" max="16" width="23.5703125" customWidth="1"/>
+    <col min="16" max="16" width="23.5546875" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" customWidth="1"/>
-    <col min="19" max="19" width="18.85546875" customWidth="1"/>
-    <col min="20" max="20" width="22.140625" customWidth="1"/>
-    <col min="21" max="21" width="24.42578125" customWidth="1"/>
-    <col min="22" max="22" width="22.140625" customWidth="1"/>
-    <col min="23" max="23" width="24.42578125" customWidth="1"/>
-    <col min="24" max="24" width="20.5703125" customWidth="1"/>
-    <col min="25" max="25" width="23.5703125" customWidth="1"/>
-    <col min="26" max="26" width="10.85546875" customWidth="1"/>
-    <col min="27" max="27" width="9.85546875" customWidth="1"/>
-    <col min="28" max="28" width="21.140625" customWidth="1"/>
-    <col min="29" max="29" width="27.140625" customWidth="1"/>
-    <col min="30" max="30" width="12.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.44140625" customWidth="1"/>
+    <col min="19" max="19" width="18.88671875" customWidth="1"/>
+    <col min="20" max="20" width="22.109375" customWidth="1"/>
+    <col min="21" max="21" width="24.44140625" customWidth="1"/>
+    <col min="22" max="22" width="22.109375" customWidth="1"/>
+    <col min="23" max="23" width="24.44140625" customWidth="1"/>
+    <col min="24" max="24" width="20.5546875" customWidth="1"/>
+    <col min="25" max="25" width="23.5546875" customWidth="1"/>
+    <col min="26" max="26" width="10.88671875" customWidth="1"/>
+    <col min="27" max="27" width="9.88671875" customWidth="1"/>
+    <col min="28" max="28" width="21.109375" customWidth="1"/>
+    <col min="29" max="29" width="27.109375" customWidth="1"/>
+    <col min="30" max="30" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="34"/>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41" t="s">
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="K1" s="41" t="s">
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="K1" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="L1" s="41"/>
-      <c r="P1" s="40" t="s">
+      <c r="L1" s="43"/>
+      <c r="P1" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
       <c r="S1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="Z1" s="40" t="s">
+      <c r="Z1" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="AA1" s="40"/>
+      <c r="AA1" s="42"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="34"/>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
     </row>
-    <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+    <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="P3" s="39" t="s">
+      <c r="P3" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39" t="s">
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="T3" s="39" t="s">
+      <c r="T3" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="U3" s="39" t="s">
+      <c r="U3" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="X3" s="39" t="s">
+      <c r="X3" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="Z3" s="48" t="s">
+      <c r="Z3" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="AA3" s="48">
+      <c r="AA3" s="21">
         <f>SUM(Z17+Z14+Z18+Z19+Z21)</f>
         <v>22000</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A4" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="39"/>
-      <c r="X4" s="39"/>
-      <c r="Z4" s="49" t="s">
+      <c r="F4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
+      <c r="X4" s="44"/>
+      <c r="Z4" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="AA4" s="49">
-        <f>SUM(Z8:Z29)-AA3</f>
-        <v>18000</v>
+      <c r="AA4" s="41">
+        <f>SUM(Z8:Z31)-AA3</f>
+        <v>20000</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="F5" s="39"/>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="F5" s="44"/>
     </row>
-    <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+    <row r="6" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
         <v>95</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1396,7 +1391,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="28">
         <v>0</v>
       </c>
@@ -1464,8 +1459,8 @@
       <c r="AD8" s="6"/>
       <c r="AE8" s="31"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="36">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A9" s="35">
         <v>111</v>
       </c>
       <c r="B9" t="s">
@@ -1537,8 +1532,8 @@
       <c r="AD9" s="6"/>
       <c r="AE9" s="31"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A10" s="36">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A10" s="35">
         <v>118</v>
       </c>
       <c r="B10" t="s">
@@ -1586,8 +1581,8 @@
       <c r="AD10" s="6"/>
       <c r="AE10" s="31"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A11" s="38">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A11" s="37">
         <v>128</v>
       </c>
       <c r="B11" t="s">
@@ -1650,8 +1645,8 @@
       <c r="AD11" s="6"/>
       <c r="AE11" s="31"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="36">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A12" s="35">
         <v>124</v>
       </c>
       <c r="B12" t="s">
@@ -1699,7 +1694,7 @@
       <c r="AD12" s="6"/>
       <c r="AE12" s="31"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
         <v>0</v>
       </c>
@@ -1765,8 +1760,8 @@
       <c r="AD13" s="6"/>
       <c r="AE13" s="31"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="38">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A14" s="37">
         <v>17</v>
       </c>
       <c r="B14" t="s">
@@ -1836,8 +1831,8 @@
       <c r="AD14" s="6"/>
       <c r="AE14" s="31"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" s="36">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A15" s="35">
         <v>115</v>
       </c>
       <c r="B15" t="s">
@@ -1903,8 +1898,8 @@
       <c r="AD15" s="6"/>
       <c r="AE15" s="31"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="36">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A16" s="35">
         <v>119</v>
       </c>
       <c r="B16" t="s">
@@ -1976,7 +1971,7 @@
       <c r="AD16" s="6"/>
       <c r="AE16" s="31"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
         <v>0</v>
       </c>
@@ -2049,7 +2044,7 @@
       <c r="AD17" s="6"/>
       <c r="AE17" s="31"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
         <v>0</v>
       </c>
@@ -2116,8 +2111,8 @@
       <c r="AD18" s="6"/>
       <c r="AE18" s="31"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A19" s="38">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A19" s="37">
         <v>11</v>
       </c>
       <c r="B19" t="s">
@@ -2185,7 +2180,7 @@
       <c r="AD19" s="6"/>
       <c r="AE19" s="31"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
         <v>0</v>
       </c>
@@ -2250,7 +2245,7 @@
       <c r="AD20" s="6"/>
       <c r="AE20" s="31"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="28">
         <v>0</v>
       </c>
@@ -2319,7 +2314,7 @@
       <c r="AD21" s="6"/>
       <c r="AE21" s="31"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="28">
         <v>0</v>
       </c>
@@ -2390,7 +2385,7 @@
       <c r="AD22" s="6"/>
       <c r="AE22" s="31"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="28">
         <v>0</v>
       </c>
@@ -2456,8 +2451,8 @@
       <c r="AD23" s="6"/>
       <c r="AE23" s="31"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A24" s="38">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A24" s="37">
         <v>124</v>
       </c>
       <c r="B24" t="s">
@@ -2503,8 +2498,8 @@
       <c r="AD24" s="6"/>
       <c r="AE24" s="31"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A25" s="38">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A25" s="37">
         <v>131</v>
       </c>
       <c r="B25" t="s">
@@ -2552,7 +2547,7 @@
       </c>
       <c r="AE25" s="31"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" s="28">
         <v>0</v>
       </c>
@@ -2618,8 +2613,8 @@
       <c r="AD26" s="6"/>
       <c r="AE26" s="31"/>
     </row>
-    <row r="27" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="36">
+    <row r="27" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="35">
         <v>118</v>
       </c>
       <c r="B27" s="9" t="s">
@@ -2683,12 +2678,9 @@
         <v>140</v>
       </c>
       <c r="AD27" s="6"/>
-      <c r="AE27" s="31">
-        <f ca="1">B8:AE27</f>
-        <v>0</v>
-      </c>
+      <c r="AE27" s="31"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f>N28</f>
         <v>117</v>
@@ -2737,132 +2729,112 @@
       <c r="AA28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB28" s="42">
+      <c r="AB28" s="38">
         <v>43472.469039351854</v>
       </c>
-      <c r="AC28" s="35"/>
+      <c r="AC28" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="AD28" s="14"/>
       <c r="AE28" s="30" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A29" s="36">
-        <f t="shared" ref="A29:A31" si="0">N29</f>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A29" s="35">
+        <f t="shared" ref="A29:A30" si="0">N29</f>
         <v>127</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29">
         <v>6666</v>
       </c>
-      <c r="D29" s="43" t="s">
+      <c r="D29" t="s">
         <v>149</v>
       </c>
-      <c r="E29" s="44"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="43">
+      <c r="E29" s="15"/>
+      <c r="N29">
         <v>127</v>
       </c>
-      <c r="O29" s="43" t="s">
+      <c r="O29" t="s">
         <v>24</v>
       </c>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="44"/>
-      <c r="R29" s="44"/>
-      <c r="S29" s="43"/>
-      <c r="T29" s="43"/>
-      <c r="U29" s="43"/>
-      <c r="V29" s="43"/>
-      <c r="W29" s="43"/>
-      <c r="X29" s="43" t="s">
+      <c r="P29" s="16"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="X29" t="s">
         <v>87</v>
       </c>
-      <c r="Y29" s="43" t="s">
+      <c r="Y29" t="s">
         <v>88</v>
       </c>
-      <c r="Z29" s="43">
+      <c r="Z29">
         <v>1500</v>
       </c>
-      <c r="AA29" s="43" t="s">
+      <c r="AA29" t="s">
         <v>26</v>
       </c>
       <c r="AB29" s="7">
         <v>43472.469039351854</v>
       </c>
-      <c r="AC29" s="28"/>
+      <c r="AC29" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="AD29" s="6"/>
       <c r="AE29" s="31" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A30" s="36">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A30" s="35">
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C30">
         <v>6666</v>
       </c>
-      <c r="D30" s="44" t="s">
+      <c r="D30" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="E30" s="44"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="43">
+      <c r="E30" s="15"/>
+      <c r="N30">
         <v>130</v>
       </c>
-      <c r="O30" s="43" t="s">
+      <c r="O30" t="s">
         <v>24</v>
       </c>
-      <c r="P30" s="45"/>
-      <c r="Q30" s="44"/>
-      <c r="R30" s="44"/>
-      <c r="S30" s="43"/>
-      <c r="T30" s="43"/>
-      <c r="U30" s="43"/>
-      <c r="V30" s="43"/>
-      <c r="W30" s="43"/>
-      <c r="X30" s="43" t="s">
+      <c r="P30" s="16"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="X30" t="s">
         <v>87</v>
       </c>
-      <c r="Y30" s="43" t="s">
+      <c r="Y30" t="s">
         <v>88</v>
       </c>
-      <c r="Z30" s="43">
+      <c r="Z30">
         <v>2000</v>
       </c>
-      <c r="AA30" s="43" t="s">
+      <c r="AA30" t="s">
         <v>26</v>
       </c>
       <c r="AB30" s="7">
         <v>43472.469039351854</v>
       </c>
-      <c r="AC30" s="28"/>
+      <c r="AC30" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="AD30" s="6"/>
       <c r="AE30" s="31" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="29"/>
       <c r="B31" s="26" t="s">
         <v>145</v>
@@ -2911,7 +2883,9 @@
       <c r="AB31" s="13">
         <v>43472.469039351854</v>
       </c>
-      <c r="AC31" s="29"/>
+      <c r="AC31" s="26" t="s">
+        <v>140</v>
+      </c>
       <c r="AD31" s="26"/>
       <c r="AE31" s="32" t="s">
         <v>129</v>
@@ -2922,18 +2896,18 @@
     <sortCondition ref="AB7"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="P3:R4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="S3:S4"/>
     <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="P3:R4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="S3:S4"/>
   </mergeCells>
   <conditionalFormatting sqref="O7:O30 O36:O1048576 O1:O4">
     <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="outgoing">

</xml_diff>